<commit_message>
Aba Compra de Mercadorias (1 de 2) - Projeto
</commit_message>
<xml_diff>
--- a/Projeto/Controle+Mercado_inicial.xlsx
+++ b/Projeto/Controle+Mercado_inicial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAN\Desktop\Curso-Excel\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A38D55-F821-4402-A510-F91926455FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6402859-0D21-4506-9173-A65C67EE53AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="Vendas" sheetId="3" r:id="rId7"/>
     <sheet name="cálculos" sheetId="5" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">cálculos!$M$6:$P$6</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
   <si>
     <t>Resultados</t>
   </si>
@@ -163,9 +166,6 @@
     <t>Couve</t>
   </si>
   <si>
-    <t>Pão</t>
-  </si>
-  <si>
     <t>Caixa de Fósforo</t>
   </si>
   <si>
@@ -221,13 +221,110 @@
   </si>
   <si>
     <t>Total de Despesas de Funcionamento</t>
+  </si>
+  <si>
+    <t>Compras de Mercadoria</t>
+  </si>
+  <si>
+    <t>Fornecedor</t>
+  </si>
+  <si>
+    <t>Mercadoria</t>
+  </si>
+  <si>
+    <t>Medida</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Preço Unitário</t>
+  </si>
+  <si>
+    <t>Desconto</t>
+  </si>
+  <si>
+    <t>Valor Pago</t>
+  </si>
+  <si>
+    <t>Produtos</t>
+  </si>
+  <si>
+    <t>Preço de Compra Unitário</t>
+  </si>
+  <si>
+    <t>Preço de Venda Unitário</t>
+  </si>
+  <si>
+    <t>Unidade</t>
+  </si>
+  <si>
+    <t>Pacote</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>Leite</t>
+  </si>
+  <si>
+    <t>Litro</t>
+  </si>
+  <si>
+    <t>Lata</t>
+  </si>
+  <si>
+    <t>Barra</t>
+  </si>
+  <si>
+    <t>Maço</t>
+  </si>
+  <si>
+    <t>Pão de Forma</t>
+  </si>
+  <si>
+    <t>Refrigerante</t>
+  </si>
+  <si>
+    <t>Garrafa</t>
+  </si>
+  <si>
+    <t>Fornecedor de Verduras</t>
+  </si>
+  <si>
+    <t>Fornecedor de Grãos e Sementes</t>
+  </si>
+  <si>
+    <t>Fornecedor de Bebidas</t>
+  </si>
+  <si>
+    <t>Fornecedor de Cigarro</t>
+  </si>
+  <si>
+    <t>Fornecedor de Doces</t>
+  </si>
+  <si>
+    <t>Padaria</t>
+  </si>
+  <si>
+    <t>Fornecedor de Frango</t>
+  </si>
+  <si>
+    <t>Fornecedor de Peixe</t>
+  </si>
+  <si>
+    <t>Fornecedor de Legumes</t>
+  </si>
+  <si>
+    <t>Fornecedor de Carne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
@@ -293,11 +390,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -308,12 +406,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -767,6 +880,28 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{352720A9-1BD4-45A2-A452-63A7E6333F8F}" name="Tabela2" displayName="Tabela2" ref="B4:I28" totalsRowShown="0">
+  <autoFilter ref="B4:I28" xr:uid="{352720A9-1BD4-45A2-A452-63A7E6333F8F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:I28">
+    <sortCondition descending="1" ref="B4:B28"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{70F01BB3-039F-4F6A-9127-0FE396F11917}" name="Data" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{23FDBB76-891B-4BEF-88E5-CF45534E4FA6}" name="Fornecedor"/>
+    <tableColumn id="3" xr3:uid="{47E77675-1CB5-4223-999C-CD7D30DA4298}" name="Mercadoria"/>
+    <tableColumn id="4" xr3:uid="{50509D53-9FDE-434A-A21C-765E6322AE8A}" name="Medida"/>
+    <tableColumn id="5" xr3:uid="{FF08DCA9-D260-4B65-9D79-32D0EDA3AD9A}" name="Quantidade"/>
+    <tableColumn id="6" xr3:uid="{BDD50E25-5158-4F1F-BC90-ABBF12938393}" name="Preço Unitário" dataCellStyle="Moeda"/>
+    <tableColumn id="7" xr3:uid="{FBF94F4E-37BE-4D76-BDDD-D3C765A36413}" name="Desconto" dataCellStyle="Porcentagem"/>
+    <tableColumn id="8" xr3:uid="{AEFD3C74-15EE-4D2B-9559-6E09557523AE}" name="Valor Pago" dataDxfId="0" dataCellStyle="Moeda">
+      <calculatedColumnFormula>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -1078,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,27 +1229,27 @@
   <sheetData>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>51</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>53</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1128,7 +1263,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4">
@@ -1178,7 +1313,7 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" s="4">
         <v>1500</v>
@@ -1215,7 +1350,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="4">
         <v>800</v>
@@ -1224,7 +1359,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" s="4">
         <v>3200</v>
@@ -1233,7 +1368,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" s="4">
         <v>500</v>
@@ -1242,7 +1377,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" s="4">
         <v>800</v>
@@ -1351,7 +1486,7 @@
     </row>
     <row r="31" spans="2:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B31" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1373,124 +1508,529 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="C3:C24"/>
+  <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="2" spans="2:9" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>42190</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5" s="4">
+        <v>5</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="I5" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>237.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>42190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6">
+        <v>120</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>42189</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>150</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <v>42189</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="F8">
+        <v>150</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <v>42189</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
+        <v>42189</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <v>200</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <v>42188</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
+        <v>42188</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
+        <v>42188</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="F13">
+        <v>300</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="11">
+        <v>42188</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
+        <v>42188</v>
+      </c>
+      <c r="C15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15">
+        <v>300</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
+        <v>42188</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="11">
+        <v>42188</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <v>42188</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18">
+        <v>110</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="11">
+        <v>42188</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="11">
+        <v>42187</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20">
+        <v>300</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
+        <v>42187</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="F21">
+        <v>150</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="11">
+        <v>42187</v>
+      </c>
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22">
+        <v>150</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
+        <v>42187</v>
+      </c>
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="F23">
+        <v>150</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
+        <v>42187</v>
+      </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24">
+        <v>100</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <v>42187</v>
+      </c>
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="F25">
+        <v>80</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <v>42187</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>48</v>
+      <c r="F26">
+        <v>100</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="11"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="4">
+        <f>Tabela2[[#This Row],[Quantidade]]*Tabela2[[#This Row],[Preço Unitário]]*(1-Tabela2[[#This Row],[Desconto]])</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6E8ACD56-AA8F-4C77-951B-4A6EB0C3FEA7}">
+          <x14:formula1>
+            <xm:f>cálculos!$M$7:$M$30</xm:f>
+          </x14:formula1>
+          <xm:sqref>D27:D28</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1576,14 +2116,376 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="M6:P30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="9">
+        <v>2.84</v>
+      </c>
+      <c r="O7" s="9">
+        <v>2.99</v>
+      </c>
+      <c r="P7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="9">
+        <v>1.06</v>
+      </c>
+      <c r="O8" s="9">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="P8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="9">
+        <v>2.34</v>
+      </c>
+      <c r="O9" s="9">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="P9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="9">
+        <v>1.85</v>
+      </c>
+      <c r="O10" s="9">
+        <v>1.99</v>
+      </c>
+      <c r="P10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" s="9">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="O11" s="9">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="P11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" s="9">
+        <v>0.74</v>
+      </c>
+      <c r="O12" s="9">
+        <v>0.79</v>
+      </c>
+      <c r="P12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="9">
+        <v>14.47</v>
+      </c>
+      <c r="O13" s="9">
+        <v>15.9</v>
+      </c>
+      <c r="P13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14" s="9">
+        <v>3.63</v>
+      </c>
+      <c r="O14" s="9">
+        <v>3.99</v>
+      </c>
+      <c r="P14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="O15" s="9">
+        <v>2.19</v>
+      </c>
+      <c r="P15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" s="9">
+        <v>4.54</v>
+      </c>
+      <c r="O16" s="9">
+        <v>4.99</v>
+      </c>
+      <c r="P16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" s="9">
+        <v>6.35</v>
+      </c>
+      <c r="O17" s="9">
+        <v>6.75</v>
+      </c>
+      <c r="P17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>42</v>
+      </c>
+      <c r="N18" s="9">
+        <v>2.37</v>
+      </c>
+      <c r="O18" s="9">
+        <v>2.6</v>
+      </c>
+      <c r="P18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="9">
+        <v>4.07</v>
+      </c>
+      <c r="O19" s="9">
+        <v>4.28</v>
+      </c>
+      <c r="P19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>32</v>
+      </c>
+      <c r="N20" s="9">
+        <v>6.42</v>
+      </c>
+      <c r="O20" s="9">
+        <v>6.98</v>
+      </c>
+      <c r="P20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>76</v>
+      </c>
+      <c r="N21" s="9">
+        <v>1.37</v>
+      </c>
+      <c r="O21" s="9">
+        <v>1.49</v>
+      </c>
+      <c r="P21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>81</v>
+      </c>
+      <c r="N22" s="9">
+        <v>2.63</v>
+      </c>
+      <c r="O22" s="9">
+        <v>2.89</v>
+      </c>
+      <c r="P22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23" s="9">
+        <v>22.23</v>
+      </c>
+      <c r="O23" s="9">
+        <v>23.9</v>
+      </c>
+      <c r="P23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" s="9">
+        <v>23.83</v>
+      </c>
+      <c r="O24" s="9">
+        <v>25.9</v>
+      </c>
+      <c r="P24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>82</v>
+      </c>
+      <c r="N25" s="9">
+        <v>2.17</v>
+      </c>
+      <c r="O25" s="9">
+        <v>2.39</v>
+      </c>
+      <c r="P25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>36</v>
+      </c>
+      <c r="N26" s="9">
+        <v>3.21</v>
+      </c>
+      <c r="O26" s="9">
+        <v>3.45</v>
+      </c>
+      <c r="P26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>29</v>
+      </c>
+      <c r="N27" s="9">
+        <v>5.35</v>
+      </c>
+      <c r="O27" s="9">
+        <v>5.82</v>
+      </c>
+      <c r="P27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>38</v>
+      </c>
+      <c r="N28" s="9">
+        <v>9.1</v>
+      </c>
+      <c r="O28" s="9">
+        <v>9.58</v>
+      </c>
+      <c r="P28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>35</v>
+      </c>
+      <c r="N29" s="9">
+        <v>26.01</v>
+      </c>
+      <c r="O29" s="9">
+        <v>29.9</v>
+      </c>
+      <c r="P29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>41</v>
+      </c>
+      <c r="N30" s="9">
+        <v>46.67</v>
+      </c>
+      <c r="O30" s="9">
+        <v>54.9</v>
+      </c>
+      <c r="P30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="M6:P6" xr:uid="{00000000-0001-0000-0700-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M7:P30">
+      <sortCondition ref="M6"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>